<commit_message>
Imagenes de sistema completo
</commit_message>
<xml_diff>
--- a/matlab_ubol/analisis_fotorres/fotorres_values.xlsx
+++ b/matlab_ubol/analisis_fotorres/fotorres_values.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_old\proyecto_ubolometro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_old\proyecto_ubolometro\matlab_ubol\analisis_fotorres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FCBAB0A-D5F8-477E-920A-BDB8AB5E591E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0722085E-284C-4A29-AD2E-99796207270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6B4B556-C4BA-4E77-9412-D36EDE38B799}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Vfuente</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>6.25 - 6.4k</t>
+  </si>
+  <si>
+    <t>(1,1)</t>
+  </si>
+  <si>
+    <t>(1,2)</t>
+  </si>
+  <si>
+    <t>(2,1)</t>
+  </si>
+  <si>
+    <t>(2,2)</t>
+  </si>
+  <si>
+    <t>Posición</t>
+  </si>
+  <si>
+    <t>29k - 31k</t>
+  </si>
+  <si>
+    <t>16k - 17k</t>
+  </si>
+  <si>
+    <t>11k - 12k</t>
+  </si>
+  <si>
+    <t>8k - 9k</t>
   </si>
 </sst>
 </file>
@@ -96,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +145,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,15 +197,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -175,10 +220,10 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -193,16 +238,34 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1398163-D196-4C8F-B465-0C7A0C0BC5BE}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +735,145 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="21"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>1</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="23"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>